<commit_message>
Improved gptApproval and loopAndCreate description functions
</commit_message>
<xml_diff>
--- a/job_listings_complete.xlsx
+++ b/job_listings_complete.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,37 +513,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4077815821</t>
+          <t>4082263309</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Full Stack Developer – WordPress</t>
+          <t>Frontend Developer</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4077815821</t>
+          <t>https://www.linkedin.com/jobs/view/4082263309</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NLvYseEEYpHKJOvp5tvCSQ==</t>
+          <t>CHFZ0O2Zz5HJxmdHgCyYOw==</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>51935941</t>
+          <t>393453653</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Fulcrum</t>
+          <t>PLAYA3ULL GAMES</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Sydney, New South Wales, Australia (On-site)</t>
+          <t>Australia (Remote)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2024-11-19 03:28:45 +0000 UTC</t>
+          <t>2024-11-24 11:43:32 +0000 UTC</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -564,7 +564,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -574,59 +574,55 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2024-11-19T04:47:32.834Z</t>
+          <t>2024-11-25T08:12:03.032Z</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2024-11-19T04:47:52.265Z</t>
+          <t>2024-11-25T08:39:42.219Z</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4075202395</t>
+          <t>4081862436</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sofware Engineer - Angular/Full Stack</t>
+          <t>Full Stack Developer - Freelance</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4075202395</t>
+          <t>https://www.linkedin.com/jobs/view/4081862436</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>NLvYseEEYpHKJOvp5tvCSQ==</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>89388788</t>
-        </is>
-      </c>
+          <t>CHFZ0O2Zz5HJxmdHgCyYOw==</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>NCS Group Australia</t>
+          <t>Twine</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Sydney, New South Wales, Australia (On-site)</t>
+          <t>Australia (Remote)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2024-11-15 05:49:54 +0000 UTC</t>
+          <t>2024-11-21 12:30:39 +0000 UTC</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -637,7 +633,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -647,59 +643,59 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2024-11-19T04:47:32.884Z</t>
+          <t>2024-11-25T08:12:03.074Z</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2024-11-19T04:50:56.636Z</t>
+          <t>2024-11-25T08:39:45.641Z</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4072427627</t>
+          <t>4082423281</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Full Stack Engineer </t>
+          <t>React Developer</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4072427627</t>
+          <t>https://www.linkedin.com/jobs/view/4082423281</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NLvYseEEYpHKJOvp5tvCSQ==</t>
+          <t>CHFZ0O2Zz5HJxmdHgCyYOw==</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>118890771</t>
+          <t>856942361</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Stealth Startup</t>
+          <t>Renaissance InfoSystems</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Australia (Remote)</t>
+          <t>Sydney, New South Wales, Australia (Hybrid)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2024-11-12 09:35:13 +0000 UTC</t>
+          <t>2024-11-25 01:04:25 +0000 UTC</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -710,7 +706,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -720,227 +716,12 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2024-11-19T04:47:32.902Z</t>
+          <t>2024-11-25T08:12:02.989Z</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2024-11-19T04:51:09.997Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4073550849</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Full Stack Software Engineer (iGaming/Online Casino)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4073550849</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>NLvYseEEYpHKJOvp5tvCSQ==</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Everyrealm Inc.</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Australia (Remote)</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2024-11-10 12:15:07 +0000 UTC</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>2024-11-19T04:47:32.918Z</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>2024-11-19T04:51:21.808Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>4055042300</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Full Stack Developer</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4055042300</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>RJjOXmBcY1obnGgVs23G4w==</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>949464799</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Interface Agency Australia</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Sydney, New South Wales, Australia (On-site)</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2024-10-22 03:01:58 +0000 UTC</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>2024-11-19T04:47:32.995Z</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>2024-11-19T04:52:47.939Z</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>4032617678</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Full stack developer - React Python AWS</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/view/4032617678</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>RJjOXmBcY1obnGgVs23G4w==</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>557486138</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Infosys</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Sydney, New South Wales, Australia (Hybrid)</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2024-09-25 09:16:03 +0000 UTC</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>2024-11-19T04:47:32.997Z</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>2024-11-19T04:52:50.422Z</t>
+          <t>2024-11-25T08:39:38.684Z</t>
         </is>
       </c>
     </row>

</xml_diff>